<commit_message>
Replacing VLOOKUPS with flat data
</commit_message>
<xml_diff>
--- a/Azure Security Benchmark/2.0/asb_v2_mapping_to_nist_SP800-53_r4.xlsx
+++ b/Azure Security Benchmark/2.0/asb_v2_mapping_to_nist_SP800-53_r4.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C7A8DC-5A7A-4F2E-A17F-3B90EE6D5C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828CFF80-AE79-488F-98D7-038AE72CAB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0D791638-282F-48A1-930E-047A9FDA6B88}"/>
   </bookViews>
@@ -11,9 +11,6 @@
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
     <sheet name="NIST_ASB_reverse_mapping" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NIST_ASB_reverse_mapping!$A$1:$P$298</definedName>
   </definedNames>
@@ -6115,847 +6112,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instruction"/>
-      <sheetName val="NIST_ASB_reverse_mapping"/>
-      <sheetName val="CIS_ASB_reverse_mapping"/>
-      <sheetName val="Sheet10"/>
-      <sheetName val="Sheet8"/>
-      <sheetName val="Sheet7"/>
-      <sheetName val="Examples"/>
-      <sheetName val="NIST-ASB Mapping"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Mapping_missing"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>NIST
-800-53 Control #</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>AC-17</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>AC-2</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>AC-3</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>AC-4</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>AC-5</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>AC-7</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>AU</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>AU-11</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>AU-12</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>AU-3</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>AU-6</v>
-          </cell>
-          <cell r="B12" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>AU-8</v>
-          </cell>
-          <cell r="B13" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>CA</v>
-          </cell>
-          <cell r="B14" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>CA-2</v>
-          </cell>
-          <cell r="B15" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>CA-3</v>
-          </cell>
-          <cell r="B16" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>CA-8</v>
-          </cell>
-          <cell r="B17" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>CM</v>
-          </cell>
-          <cell r="B18" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>CM-10</v>
-          </cell>
-          <cell r="B19" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>CM-11</v>
-          </cell>
-          <cell r="B20" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>CM-2</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>CM-6</v>
-          </cell>
-          <cell r="B22" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>CM-7</v>
-          </cell>
-          <cell r="B23" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>CM-8</v>
-          </cell>
-          <cell r="B24" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>CP</v>
-          </cell>
-          <cell r="B25" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>CP-2</v>
-          </cell>
-          <cell r="B26" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>CP-4</v>
-          </cell>
-          <cell r="B27" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>CP-6</v>
-          </cell>
-          <cell r="B28" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>CP-9</v>
-          </cell>
-          <cell r="B29" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>IA-2</v>
-          </cell>
-          <cell r="B30" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>IA-4</v>
-          </cell>
-          <cell r="B31" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>IA-5</v>
-          </cell>
-          <cell r="B32" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>IA-8</v>
-          </cell>
-          <cell r="B33" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>IA-9</v>
-          </cell>
-          <cell r="B34" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>IR</v>
-          </cell>
-          <cell r="B35" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>IR-4</v>
-          </cell>
-          <cell r="B36" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>IR-5</v>
-          </cell>
-          <cell r="B37" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>IR-6</v>
-          </cell>
-          <cell r="B38" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>IR-8</v>
-          </cell>
-          <cell r="B39" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>MA-4</v>
-          </cell>
-          <cell r="B40" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>PL</v>
-          </cell>
-          <cell r="B41" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>PM</v>
-          </cell>
-          <cell r="B42" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>PM-10</v>
-          </cell>
-          <cell r="B43" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>PM-5</v>
-          </cell>
-          <cell r="B44" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>RA</v>
-          </cell>
-          <cell r="B45" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>RA-5</v>
-          </cell>
-          <cell r="B46" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>SC</v>
-          </cell>
-          <cell r="B47" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>SC-11</v>
-          </cell>
-          <cell r="B48" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>SC-12</v>
-          </cell>
-          <cell r="B49" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>SC-20</v>
-          </cell>
-          <cell r="B50" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>SC-21</v>
-          </cell>
-          <cell r="B51" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>SC-28</v>
-          </cell>
-          <cell r="B52" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>SC-3</v>
-          </cell>
-          <cell r="B53" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>SC-5</v>
-          </cell>
-          <cell r="B54" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>SC-7</v>
-          </cell>
-          <cell r="B55" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>SC-8</v>
-          </cell>
-          <cell r="B56" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>SI-2</v>
-          </cell>
-          <cell r="B57" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>SI-3</v>
-          </cell>
-          <cell r="B58" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>SI-4</v>
-          </cell>
-          <cell r="B59" t="str">
-            <v>X</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61"/>
-        </row>
-        <row r="62">
-          <cell r="A62"/>
-        </row>
-        <row r="63">
-          <cell r="A63"/>
-        </row>
-        <row r="64">
-          <cell r="A64"/>
-        </row>
-        <row r="65">
-          <cell r="A65"/>
-        </row>
-        <row r="66">
-          <cell r="A66"/>
-        </row>
-        <row r="67">
-          <cell r="A67"/>
-        </row>
-        <row r="68">
-          <cell r="A68"/>
-        </row>
-        <row r="69">
-          <cell r="A69"/>
-        </row>
-        <row r="70">
-          <cell r="A70"/>
-        </row>
-        <row r="71">
-          <cell r="A71"/>
-        </row>
-        <row r="72">
-          <cell r="A72"/>
-        </row>
-        <row r="73">
-          <cell r="A73"/>
-        </row>
-        <row r="74">
-          <cell r="A74"/>
-        </row>
-        <row r="75">
-          <cell r="A75"/>
-        </row>
-        <row r="76">
-          <cell r="A76"/>
-        </row>
-        <row r="77">
-          <cell r="A77"/>
-        </row>
-        <row r="78">
-          <cell r="A78"/>
-        </row>
-        <row r="79">
-          <cell r="A79"/>
-        </row>
-        <row r="80">
-          <cell r="A80"/>
-        </row>
-        <row r="81">
-          <cell r="A81"/>
-        </row>
-        <row r="82">
-          <cell r="A82"/>
-        </row>
-        <row r="83">
-          <cell r="A83"/>
-        </row>
-        <row r="84">
-          <cell r="A84"/>
-        </row>
-        <row r="85">
-          <cell r="A85"/>
-        </row>
-        <row r="86">
-          <cell r="A86"/>
-        </row>
-        <row r="87">
-          <cell r="A87"/>
-        </row>
-        <row r="88">
-          <cell r="A88"/>
-        </row>
-        <row r="89">
-          <cell r="A89"/>
-        </row>
-        <row r="90">
-          <cell r="A90"/>
-        </row>
-        <row r="91">
-          <cell r="A91"/>
-        </row>
-        <row r="92">
-          <cell r="A92"/>
-        </row>
-        <row r="93">
-          <cell r="A93"/>
-        </row>
-        <row r="94">
-          <cell r="A94"/>
-        </row>
-        <row r="95">
-          <cell r="A95"/>
-        </row>
-        <row r="96">
-          <cell r="A96"/>
-        </row>
-        <row r="97">
-          <cell r="A97"/>
-        </row>
-        <row r="98">
-          <cell r="A98"/>
-        </row>
-        <row r="99">
-          <cell r="A99"/>
-        </row>
-        <row r="100">
-          <cell r="A100"/>
-        </row>
-        <row r="101">
-          <cell r="A101"/>
-        </row>
-        <row r="102">
-          <cell r="A102"/>
-        </row>
-        <row r="103">
-          <cell r="A103"/>
-        </row>
-        <row r="104">
-          <cell r="A104"/>
-        </row>
-        <row r="105">
-          <cell r="A105"/>
-        </row>
-        <row r="106">
-          <cell r="A106"/>
-        </row>
-        <row r="107">
-          <cell r="A107"/>
-        </row>
-        <row r="108">
-          <cell r="A108"/>
-        </row>
-        <row r="109">
-          <cell r="A109"/>
-        </row>
-        <row r="110">
-          <cell r="A110"/>
-        </row>
-        <row r="111">
-          <cell r="A111"/>
-        </row>
-        <row r="112">
-          <cell r="A112"/>
-        </row>
-        <row r="113">
-          <cell r="A113"/>
-        </row>
-        <row r="114">
-          <cell r="A114"/>
-        </row>
-        <row r="115">
-          <cell r="A115"/>
-        </row>
-        <row r="116">
-          <cell r="A116"/>
-        </row>
-        <row r="117">
-          <cell r="A117"/>
-        </row>
-        <row r="118">
-          <cell r="A118"/>
-        </row>
-        <row r="119">
-          <cell r="A119"/>
-        </row>
-        <row r="120">
-          <cell r="A120"/>
-        </row>
-        <row r="121">
-          <cell r="A121"/>
-        </row>
-        <row r="122">
-          <cell r="A122"/>
-        </row>
-        <row r="123">
-          <cell r="A123"/>
-        </row>
-        <row r="124">
-          <cell r="A124"/>
-        </row>
-        <row r="125">
-          <cell r="A125"/>
-        </row>
-        <row r="126">
-          <cell r="A126"/>
-        </row>
-        <row r="127">
-          <cell r="A127"/>
-        </row>
-        <row r="128">
-          <cell r="A128"/>
-        </row>
-        <row r="129">
-          <cell r="A129"/>
-        </row>
-        <row r="130">
-          <cell r="A130"/>
-        </row>
-        <row r="131">
-          <cell r="A131"/>
-        </row>
-        <row r="132">
-          <cell r="A132"/>
-        </row>
-        <row r="133">
-          <cell r="A133"/>
-        </row>
-        <row r="134">
-          <cell r="A134"/>
-        </row>
-        <row r="135">
-          <cell r="A135"/>
-        </row>
-        <row r="136">
-          <cell r="A136"/>
-        </row>
-        <row r="137">
-          <cell r="A137"/>
-        </row>
-        <row r="138">
-          <cell r="A138"/>
-        </row>
-        <row r="139">
-          <cell r="A139"/>
-        </row>
-        <row r="140">
-          <cell r="A140"/>
-        </row>
-        <row r="141">
-          <cell r="A141"/>
-        </row>
-        <row r="142">
-          <cell r="A142"/>
-        </row>
-        <row r="143">
-          <cell r="A143"/>
-        </row>
-        <row r="144">
-          <cell r="A144"/>
-        </row>
-        <row r="145">
-          <cell r="A145"/>
-        </row>
-        <row r="146">
-          <cell r="A146"/>
-        </row>
-        <row r="147">
-          <cell r="A147"/>
-        </row>
-        <row r="148">
-          <cell r="A148"/>
-        </row>
-        <row r="149">
-          <cell r="A149"/>
-        </row>
-        <row r="150">
-          <cell r="A150"/>
-        </row>
-        <row r="151">
-          <cell r="A151"/>
-        </row>
-        <row r="152">
-          <cell r="A152"/>
-        </row>
-        <row r="153">
-          <cell r="A153"/>
-        </row>
-        <row r="154">
-          <cell r="A154"/>
-        </row>
-        <row r="155">
-          <cell r="A155"/>
-        </row>
-        <row r="156">
-          <cell r="A156"/>
-        </row>
-        <row r="157">
-          <cell r="A157"/>
-        </row>
-        <row r="158">
-          <cell r="A158"/>
-        </row>
-        <row r="159">
-          <cell r="A159"/>
-        </row>
-        <row r="160">
-          <cell r="A160"/>
-        </row>
-        <row r="161">
-          <cell r="A161"/>
-        </row>
-        <row r="162">
-          <cell r="A162"/>
-        </row>
-        <row r="163">
-          <cell r="A163"/>
-        </row>
-        <row r="164">
-          <cell r="A164"/>
-        </row>
-        <row r="165">
-          <cell r="A165"/>
-        </row>
-        <row r="166">
-          <cell r="A166"/>
-        </row>
-        <row r="167">
-          <cell r="A167"/>
-        </row>
-        <row r="168">
-          <cell r="A168"/>
-        </row>
-        <row r="169">
-          <cell r="A169"/>
-        </row>
-        <row r="170">
-          <cell r="A170"/>
-        </row>
-        <row r="171">
-          <cell r="A171"/>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7436,8 +6592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32883A0-DE69-4048-BA01-05195A615D42}">
   <dimension ref="A1:Q298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J180" sqref="J180"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15944,7 +15100,6 @@
         <v>29</v>
       </c>
       <c r="K184" s="13" t="e">
-        <f>VLOOKUP(C184,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L184" s="14" t="s">
@@ -15992,7 +15147,6 @@
         <v>29</v>
       </c>
       <c r="K185" s="13" t="e">
-        <f>VLOOKUP(C185,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L185" s="14" t="s">
@@ -16040,7 +15194,6 @@
         <v>29</v>
       </c>
       <c r="K186" s="13" t="e">
-        <f>VLOOKUP(C186,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L186" s="14" t="s">
@@ -16088,7 +15241,6 @@
         <v>29</v>
       </c>
       <c r="K187" s="13" t="e">
-        <f>VLOOKUP(C187,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L187" s="14" t="s">
@@ -16136,7 +15288,6 @@
         <v>29</v>
       </c>
       <c r="K188" s="13" t="e">
-        <f>VLOOKUP(C188,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L188" s="14" t="s">
@@ -16742,7 +15893,6 @@
         <v>29</v>
       </c>
       <c r="K201" s="13" t="e">
-        <f>VLOOKUP(C201,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L201" s="14" t="s">
@@ -16790,7 +15940,6 @@
         <v>29</v>
       </c>
       <c r="K202" s="13" t="e">
-        <f>VLOOKUP(C202,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L202" s="14" t="s">
@@ -17017,7 +16166,6 @@
         <v>29</v>
       </c>
       <c r="K207" s="13" t="e">
-        <f>VLOOKUP(C207,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L207" s="14" t="s">
@@ -17062,7 +16210,6 @@
         <v>29</v>
       </c>
       <c r="K208" s="13" t="e">
-        <f>VLOOKUP(C208,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L208" s="14" t="s">
@@ -17110,7 +16257,6 @@
         <v>29</v>
       </c>
       <c r="K209" s="13" t="e">
-        <f>VLOOKUP(C209,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L209" s="14" t="s">
@@ -17202,7 +16348,6 @@
         <v>29</v>
       </c>
       <c r="K211" s="13" t="e">
-        <f>VLOOKUP(C211,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L211" s="14" t="s">
@@ -17250,7 +16395,6 @@
         <v>29</v>
       </c>
       <c r="K212" s="13" t="e">
-        <f>VLOOKUP(C212,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L212" s="14" t="s">
@@ -17298,7 +16442,6 @@
         <v>29</v>
       </c>
       <c r="K213" s="13" t="e">
-        <f>VLOOKUP(C213,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L213" s="14" t="s">
@@ -17569,7 +16712,6 @@
         <v>29</v>
       </c>
       <c r="K219" s="13" t="e">
-        <f>VLOOKUP(C219,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L219" s="14" t="s">
@@ -17617,7 +16759,6 @@
         <v>29</v>
       </c>
       <c r="K220" s="13" t="e">
-        <f>VLOOKUP(C220,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L220" s="14" t="s">
@@ -17662,7 +16803,6 @@
         <v>29</v>
       </c>
       <c r="K221" s="13" t="e">
-        <f>VLOOKUP(C221,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L221" s="14" t="s">
@@ -17710,7 +16850,6 @@
         <v>29</v>
       </c>
       <c r="K222" s="13" t="e">
-        <f>VLOOKUP(C222,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L222" s="14" t="s">
@@ -17755,7 +16894,6 @@
         <v>29</v>
       </c>
       <c r="K223" s="13" t="e">
-        <f>VLOOKUP(C223,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L223" s="14" t="s">
@@ -17803,7 +16941,6 @@
         <v>29</v>
       </c>
       <c r="K224" s="13" t="e">
-        <f>VLOOKUP(C224,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L224" s="14" t="s">
@@ -17851,7 +16988,6 @@
         <v>29</v>
       </c>
       <c r="K225" s="13" t="e">
-        <f>VLOOKUP(C225,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L225" s="14" t="s">
@@ -17896,7 +17032,6 @@
         <v>29</v>
       </c>
       <c r="K226" s="13" t="e">
-        <f>VLOOKUP(C226,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L226" s="14" t="s">
@@ -17941,7 +17076,6 @@
         <v>29</v>
       </c>
       <c r="K227" s="13" t="e">
-        <f>VLOOKUP(C227,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L227" s="14" t="s">
@@ -17986,7 +17120,6 @@
         <v>29</v>
       </c>
       <c r="K228" s="13" t="e">
-        <f>VLOOKUP(C228,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L228" s="14" t="s">
@@ -18034,7 +17167,6 @@
         <v>29</v>
       </c>
       <c r="K229" s="13" t="e">
-        <f>VLOOKUP(C229,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L229" s="14" t="s">
@@ -18082,7 +17214,6 @@
         <v>29</v>
       </c>
       <c r="K230" s="13" t="e">
-        <f>VLOOKUP(C230,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L230" s="14" t="s">
@@ -18130,7 +17261,6 @@
         <v>29</v>
       </c>
       <c r="K231" s="13" t="e">
-        <f>VLOOKUP(C231,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L231" s="14" t="s">
@@ -18178,7 +17308,6 @@
         <v>29</v>
       </c>
       <c r="K232" s="13" t="e">
-        <f>VLOOKUP(C232,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L232" s="14" t="s">
@@ -18226,7 +17355,6 @@
         <v>29</v>
       </c>
       <c r="K233" s="13" t="e">
-        <f>VLOOKUP(C233,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L233" s="14" t="s">
@@ -18271,7 +17399,6 @@
         <v>29</v>
       </c>
       <c r="K234" s="13" t="e">
-        <f>VLOOKUP(C234,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L234" s="14" t="s">
@@ -18316,7 +17443,6 @@
         <v>29</v>
       </c>
       <c r="K235" s="13" t="e">
-        <f>VLOOKUP(C235,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L235" s="14" t="s">
@@ -18364,7 +17490,6 @@
         <v>29</v>
       </c>
       <c r="K236" s="13" t="e">
-        <f>VLOOKUP(C236,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L236" s="14" t="s">
@@ -18412,7 +17537,6 @@
         <v>29</v>
       </c>
       <c r="K237" s="13" t="e">
-        <f>VLOOKUP(C237,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L237" s="14" t="s">
@@ -18457,7 +17581,6 @@
         <v>29</v>
       </c>
       <c r="K238" s="13" t="e">
-        <f>VLOOKUP(C238,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L238" s="14" t="s">
@@ -18502,7 +17625,6 @@
         <v>29</v>
       </c>
       <c r="K239" s="13" t="e">
-        <f>VLOOKUP(C239,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L239" s="14" t="s">
@@ -18547,7 +17669,6 @@
         <v>29</v>
       </c>
       <c r="K240" s="13" t="e">
-        <f>VLOOKUP(C240,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L240" s="14" t="s">
@@ -18595,7 +17716,6 @@
         <v>29</v>
       </c>
       <c r="K241" s="13" t="e">
-        <f>VLOOKUP(C241,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L241" s="14" t="s">
@@ -18643,7 +17763,6 @@
         <v>29</v>
       </c>
       <c r="K242" s="13" t="e">
-        <f>VLOOKUP(C242,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L242" s="14" t="s">
@@ -18691,7 +17810,6 @@
         <v>29</v>
       </c>
       <c r="K243" s="13" t="e">
-        <f>VLOOKUP(C243,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L243" s="14" t="s">
@@ -18739,7 +17857,6 @@
         <v>29</v>
       </c>
       <c r="K244" s="13" t="e">
-        <f>VLOOKUP(C244,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L244" s="14" t="s">
@@ -18787,7 +17904,6 @@
         <v>29</v>
       </c>
       <c r="K245" s="13" t="e">
-        <f>VLOOKUP(C245,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L245" s="14" t="s">
@@ -18832,7 +17948,6 @@
         <v>29</v>
       </c>
       <c r="K246" s="13" t="e">
-        <f>VLOOKUP(C246,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L246" s="14" t="s">
@@ -19065,7 +18180,6 @@
         <v>29</v>
       </c>
       <c r="K251" s="13" t="e">
-        <f>VLOOKUP(C251,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L251" s="14" t="s">
@@ -19113,7 +18227,6 @@
         <v>29</v>
       </c>
       <c r="K252" s="13" t="e">
-        <f>VLOOKUP(C252,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L252" s="14" t="s">
@@ -19161,7 +18274,6 @@
         <v>29</v>
       </c>
       <c r="K253" s="13" t="e">
-        <f>VLOOKUP(C253,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L253" s="14" t="s">
@@ -19303,7 +18415,6 @@
         <v>29</v>
       </c>
       <c r="K256" s="13" t="e">
-        <f>VLOOKUP(C256,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L256" s="14" t="s">
@@ -19351,7 +18462,6 @@
         <v>29</v>
       </c>
       <c r="K257" s="13" t="e">
-        <f>VLOOKUP(C257,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L257" s="14" t="s">
@@ -19399,7 +18509,6 @@
         <v>29</v>
       </c>
       <c r="K258" s="13" t="e">
-        <f>VLOOKUP(C258,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L258" s="14" t="s">
@@ -19588,7 +18697,6 @@
         <v>29</v>
       </c>
       <c r="K262" s="13" t="e">
-        <f>VLOOKUP(C262,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L262" s="14" t="s">
@@ -19636,7 +18744,6 @@
         <v>29</v>
       </c>
       <c r="K263" s="13" t="e">
-        <f>VLOOKUP(C263,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L263" s="14" t="s">
@@ -19684,7 +18791,6 @@
         <v>29</v>
       </c>
       <c r="K264" s="13" t="e">
-        <f>VLOOKUP(C264,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L264" s="14" t="s">
@@ -19732,7 +18838,6 @@
         <v>29</v>
       </c>
       <c r="K265" s="13" t="e">
-        <f>VLOOKUP(C265,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L265" s="14" t="s">
@@ -19780,7 +18885,6 @@
         <v>29</v>
       </c>
       <c r="K266" s="13" t="e">
-        <f>VLOOKUP(C266,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L266" s="14" t="s">
@@ -19825,7 +18929,6 @@
         <v>29</v>
       </c>
       <c r="K267" s="13" t="e">
-        <f>VLOOKUP(C267,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L267" s="14" t="s">
@@ -19873,7 +18976,6 @@
         <v>29</v>
       </c>
       <c r="K268" s="13" t="e">
-        <f>VLOOKUP(C268,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L268" s="14" t="s">
@@ -19918,7 +19020,6 @@
         <v>29</v>
       </c>
       <c r="K269" s="13" t="e">
-        <f>VLOOKUP(C269,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L269" s="14" t="s">
@@ -19963,7 +19064,6 @@
         <v>29</v>
       </c>
       <c r="K270" s="13" t="e">
-        <f>VLOOKUP(C270,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L270" s="14" t="s">
@@ -20055,7 +19155,6 @@
         <v>29</v>
       </c>
       <c r="K272" s="13" t="e">
-        <f>VLOOKUP(C272,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L272" s="14" t="s">
@@ -20100,7 +19199,6 @@
         <v>29</v>
       </c>
       <c r="K273" s="13" t="e">
-        <f>VLOOKUP(C273,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L273" s="14" t="s">
@@ -20145,7 +19243,6 @@
         <v>29</v>
       </c>
       <c r="K274" s="13" t="e">
-        <f>VLOOKUP(C274,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L274" s="14" t="s">
@@ -20193,7 +19290,6 @@
         <v>29</v>
       </c>
       <c r="K275" s="13" t="e">
-        <f>VLOOKUP(C275,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L275" s="14" t="s">
@@ -20241,7 +19337,6 @@
         <v>29</v>
       </c>
       <c r="K276" s="13" t="e">
-        <f>VLOOKUP(C276,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L276" s="14" t="s">
@@ -20286,7 +19381,6 @@
         <v>29</v>
       </c>
       <c r="K277" s="13" t="e">
-        <f>VLOOKUP(C277,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L277" s="14" t="s">
@@ -20331,7 +19425,6 @@
         <v>29</v>
       </c>
       <c r="K278" s="13" t="e">
-        <f>VLOOKUP(C278,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L278" s="14" t="s">
@@ -20376,7 +19469,6 @@
         <v>29</v>
       </c>
       <c r="K279" s="13" t="e">
-        <f>VLOOKUP(C279,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L279" s="14" t="s">
@@ -20424,7 +19516,6 @@
         <v>29</v>
       </c>
       <c r="K280" s="13" t="e">
-        <f>VLOOKUP(C280,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L280" s="14" t="s">
@@ -20469,7 +19560,6 @@
         <v>29</v>
       </c>
       <c r="K281" s="13" t="e">
-        <f>VLOOKUP(C281,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L281" s="14" t="s">
@@ -20517,7 +19607,6 @@
         <v>29</v>
       </c>
       <c r="K282" s="13" t="e">
-        <f>VLOOKUP(C282,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L282" s="14" t="s">
@@ -20565,7 +19654,6 @@
         <v>29</v>
       </c>
       <c r="K283" s="13" t="e">
-        <f>VLOOKUP(C283,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L283" s="14" t="s">
@@ -20613,7 +19701,6 @@
         <v>29</v>
       </c>
       <c r="K284" s="13" t="e">
-        <f>VLOOKUP(C284,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L284" s="14" t="s">
@@ -20655,7 +19742,6 @@
         <v>29</v>
       </c>
       <c r="K285" s="13" t="e">
-        <f>VLOOKUP(C285,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L285" s="14" t="s">
@@ -20700,7 +19786,6 @@
         <v>29</v>
       </c>
       <c r="K286" s="13" t="e">
-        <f>VLOOKUP(C286,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L286" s="14" t="s">
@@ -20745,7 +19830,6 @@
         <v>29</v>
       </c>
       <c r="K287" s="13" t="e">
-        <f>VLOOKUP(C287,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L287" s="14" t="s">
@@ -20790,7 +19874,6 @@
         <v>29</v>
       </c>
       <c r="K288" s="13" t="e">
-        <f>VLOOKUP(C288,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L288" s="14" t="s">
@@ -20835,7 +19918,6 @@
         <v>29</v>
       </c>
       <c r="K289" s="13" t="e">
-        <f>VLOOKUP(C289,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L289" s="14" t="s">
@@ -20883,7 +19965,6 @@
         <v>29</v>
       </c>
       <c r="K290" s="13" t="e">
-        <f>VLOOKUP(C290,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L290" s="14" t="s">
@@ -20966,7 +20047,6 @@
       <c r="G292" s="2"/>
       <c r="H292" s="2"/>
       <c r="K292" s="13" t="e">
-        <f>VLOOKUP(C292,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L292" s="14" t="s">
@@ -21005,7 +20085,6 @@
       <c r="G293" s="2"/>
       <c r="H293" s="2"/>
       <c r="K293" s="13" t="e">
-        <f>VLOOKUP(C293,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L293" s="14" t="s">
@@ -21041,7 +20120,6 @@
         <v>769</v>
       </c>
       <c r="K294" s="13" t="e">
-        <f>VLOOKUP(C294,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L294" s="14" t="s">
@@ -21077,7 +20155,6 @@
         <v>772</v>
       </c>
       <c r="K295" s="13" t="e">
-        <f>VLOOKUP(C295,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L295" s="14" t="s">
@@ -21113,7 +20190,6 @@
         <v>775</v>
       </c>
       <c r="K296" s="13" t="e">
-        <f>VLOOKUP(C296,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L296" s="14" t="s">
@@ -21149,7 +20225,6 @@
         <v>779</v>
       </c>
       <c r="K297" s="13" t="e">
-        <f>VLOOKUP(C297,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L297" s="14" t="s">
@@ -21185,7 +20260,6 @@
         <v>782</v>
       </c>
       <c r="K298" s="13" t="e">
-        <f>VLOOKUP(C298,[1]Sheet2!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="L298" s="14" t="s">

</xml_diff>